<commit_message>
Fix bug where first row of excel was not considered; Added custom test excel
</commit_message>
<xml_diff>
--- a/docs/test_excel.xlsx
+++ b/docs/test_excel.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LG4000\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LG4000\Desktop\comms\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C181C9A2-9496-49CE-B341-0764F5336093}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A40F769-332D-48B6-821D-84116913A94D}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{B3B8992A-2509-491A-9C39-2580EA4D3B1D}"/>
   </bookViews>
@@ -4112,7 +4112,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -4144,6 +4144,12 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -4461,86 +4467,86 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2CEAC2C5-08A0-40A6-93E9-BE2759C1F504}">
   <dimension ref="A1:Y147"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView tabSelected="1" zoomScale="69" workbookViewId="0">
+      <selection sqref="A1:Y1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
     <row r="1" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="2" t="s">
+      <c r="F1" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="I1" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="J1" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="K1" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="L1" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="M1" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="4" t="s">
+      <c r="N1" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="3" t="s">
+      <c r="O1" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="2" t="s">
+      <c r="P1" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="2" t="s">
+      <c r="Q1" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="R1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="S1" s="2" t="s">
+      <c r="R1" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="S1" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="T1" s="2" t="s">
+      <c r="T1" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="U1" s="2" t="s">
+      <c r="U1" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="V1" s="2" t="s">
+      <c r="V1" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="W1" s="2" t="s">
+      <c r="W1" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="X1" s="3" t="s">
+      <c r="X1" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="Y1" s="2" t="s">
+      <c r="Y1" s="16" t="s">
         <v>15</v>
       </c>
     </row>

</xml_diff>